<commit_message>
Added top 11 universities' data
</commit_message>
<xml_diff>
--- a/colleges/colleges-expanded.xlsx
+++ b/colleges/colleges-expanded.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidferrara/Documents/Clemson/The Tiger/COVID-19/Data/covid-19-data/colleges/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4C6087D-F6F3-464B-AB72-F7B86F31FC43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C57DAF61-A26F-9C49-9F7C-370623EC19BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="15740" xr2:uid="{2D8D1C12-08D3-174B-B1CF-8C89AF741EEC}"/>
+    <workbookView xWindow="11780" yWindow="0" windowWidth="17020" windowHeight="18000" xr2:uid="{2D8D1C12-08D3-174B-B1CF-8C89AF741EEC}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6871" uniqueCount="3327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6900" uniqueCount="3350">
   <si>
     <t>date</t>
   </si>
@@ -9992,35 +9993,111 @@
     <t>cumulative tests</t>
   </si>
   <si>
-    <t>cumulative negative tests</t>
-  </si>
-  <si>
     <t>since</t>
   </si>
   <si>
-    <t>cumulative positive tests</t>
-  </si>
-  <si>
-    <t>average # of tests in past-7 days</t>
-  </si>
-  <si>
-    <t>number of surveillance (asym) tests/time period</t>
-  </si>
-  <si>
     <t>student population size</t>
   </si>
   <si>
-    <t>student on-campus pop</t>
-  </si>
-  <si>
-    <t>response</t>
+    <t>July 28 2020</t>
+  </si>
+  <si>
+    <t>August 1 2020</t>
+  </si>
+  <si>
+    <t>65854 (OC)</t>
+  </si>
+  <si>
+    <t>average # of tests per day</t>
+  </si>
+  <si>
+    <t># of IU asym tests/week</t>
+  </si>
+  <si>
+    <t># of IU tests/day</t>
+  </si>
+  <si>
+    <t># of IU tests/week</t>
+  </si>
+  <si>
+    <t>OC is on-campus, since off-campus counts were unavailable</t>
+  </si>
+  <si>
+    <t>just undergrad count for student pop</t>
+  </si>
+  <si>
+    <t>June 5 2020</t>
+  </si>
+  <si>
+    <t>% of student pop positive</t>
+  </si>
+  <si>
+    <t>undergrad + grad</t>
+  </si>
+  <si>
+    <t>all students, undergrad + grad + prof</t>
+  </si>
+  <si>
+    <t>since pandemic</t>
+  </si>
+  <si>
+    <t>CU</t>
+  </si>
+  <si>
+    <t>very low test/day, could be #1 If there are cases uncounted. However, 3507 are since august 1, and clemson does not count cases since before june</t>
+  </si>
+  <si>
+    <t>cumulative student positive tests</t>
+  </si>
+  <si>
+    <t>March 18 2020</t>
+  </si>
+  <si>
+    <t>UF</t>
+  </si>
+  <si>
+    <t>UGA</t>
+  </si>
+  <si>
+    <t>F2019 student pop</t>
+  </si>
+  <si>
+    <t>August 7 2020</t>
+  </si>
+  <si>
+    <t>Penn</t>
+  </si>
+  <si>
+    <t>average/week</t>
+  </si>
+  <si>
+    <t>average/day</t>
+  </si>
+  <si>
+    <t>July 6 2020</t>
+  </si>
+  <si>
+    <t>most extensive/accessible data I've seen so far, with csv's of each day's data available</t>
+  </si>
+  <si>
+    <t>August 4 2020</t>
+  </si>
+  <si>
+    <t>UofSC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -10046,15 +10123,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -10366,10 +10447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FF24571-3CC7-D44E-AB7D-4F64C0C0547A}">
-  <dimension ref="A1:Q1713"/>
+  <dimension ref="A1:N1713"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -10381,15 +10462,13 @@
     <col min="7" max="7" width="15.6640625" customWidth="1"/>
     <col min="8" max="8" width="16.5" customWidth="1"/>
     <col min="9" max="9" width="14.5" customWidth="1"/>
-    <col min="10" max="10" width="21.83203125" customWidth="1"/>
-    <col min="11" max="11" width="22" customWidth="1"/>
-    <col min="12" max="12" width="28.1640625" customWidth="1"/>
-    <col min="13" max="13" width="41.5" customWidth="1"/>
-    <col min="14" max="15" width="20.33203125" customWidth="1"/>
-    <col min="16" max="16" width="31.5" customWidth="1"/>
+    <col min="10" max="10" width="28.6640625" customWidth="1"/>
+    <col min="11" max="11" width="28.1640625" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" customWidth="1"/>
+    <col min="13" max="13" width="23.1640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -10412,85 +10491,120 @@
         <v>3317</v>
       </c>
       <c r="H1" t="s">
-        <v>3320</v>
+        <v>3319</v>
       </c>
       <c r="I1" t="s">
         <v>3318</v>
       </c>
       <c r="J1" t="s">
-        <v>3321</v>
+        <v>3337</v>
       </c>
       <c r="K1" t="s">
-        <v>3319</v>
+        <v>3324</v>
       </c>
       <c r="L1" t="s">
-        <v>3322</v>
-      </c>
-      <c r="M1" t="s">
-        <v>3323</v>
+        <v>3320</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>3331</v>
       </c>
       <c r="N1" t="s">
-        <v>3324</v>
-      </c>
-      <c r="O1" t="s">
-        <v>3325</v>
-      </c>
-      <c r="P1" t="s">
-        <v>3326</v>
-      </c>
-      <c r="Q1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:14">
       <c r="A2" s="1">
-        <v>44112</v>
+        <v>44120</v>
       </c>
       <c r="B2" t="s">
+        <v>2654</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2659</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2660</v>
+      </c>
+      <c r="E2">
+        <v>217882</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2661</v>
+      </c>
+      <c r="G2">
+        <v>4460</v>
+      </c>
+      <c r="H2" t="s">
+        <v>3330</v>
+      </c>
+      <c r="I2">
+        <v>77914</v>
+      </c>
+      <c r="J2">
+        <v>4331</v>
+      </c>
+      <c r="K2">
+        <v>1148.5</v>
+      </c>
+      <c r="L2">
+        <v>25822</v>
+      </c>
+      <c r="M2" s="3">
+        <f>J2/L2</f>
+        <v>0.16772519556966928</v>
+      </c>
+      <c r="N2" t="s">
+        <v>3332</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="1">
+        <v>44120</v>
+      </c>
+      <c r="B3" t="s">
         <v>602</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>687</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="E2">
+      <c r="E3">
         <v>139959</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F3" t="s">
         <v>688</v>
       </c>
-      <c r="G2">
-        <v>3888</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="A3" s="1">
-        <v>44112</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2654</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2659</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2660</v>
-      </c>
-      <c r="E3">
-        <v>217882</v>
-      </c>
-      <c r="F3" t="s">
-        <v>2661</v>
-      </c>
       <c r="G3">
-        <v>3770</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
+        <v>3964</v>
+      </c>
+      <c r="H3" t="s">
+        <v>3334</v>
+      </c>
+      <c r="I3" t="s">
+        <v>1214</v>
+      </c>
+      <c r="J3">
+        <v>3964</v>
+      </c>
+      <c r="K3">
+        <v>240</v>
+      </c>
+      <c r="L3">
+        <v>38920</v>
+      </c>
+      <c r="M3" s="3">
+        <f>G3/L3</f>
+        <v>0.10184994861253854</v>
+      </c>
+      <c r="N3" t="s">
+        <v>3336</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="1">
-        <v>44112</v>
+        <v>44120</v>
       </c>
       <c r="B4" t="s">
         <v>2183</v>
@@ -10508,12 +10622,34 @@
         <v>2261</v>
       </c>
       <c r="G4">
-        <v>3051</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
+        <v>3261</v>
+      </c>
+      <c r="H4" t="s">
+        <v>3322</v>
+      </c>
+      <c r="I4">
+        <v>139665</v>
+      </c>
+      <c r="J4">
+        <v>3198</v>
+      </c>
+      <c r="K4">
+        <v>3028</v>
+      </c>
+      <c r="L4">
+        <v>61391</v>
+      </c>
+      <c r="M4" s="3">
+        <f>G4/L4</f>
+        <v>5.3118535290189117E-2</v>
+      </c>
+      <c r="N4" t="s">
+        <v>3333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="1">
-        <v>44112</v>
+        <v>44120</v>
       </c>
       <c r="B5" t="s">
         <v>3249</v>
@@ -10531,12 +10667,34 @@
         <v>3287</v>
       </c>
       <c r="G5">
-        <v>3041</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
+        <v>3219</v>
+      </c>
+      <c r="H5" t="s">
+        <v>3321</v>
+      </c>
+      <c r="I5" t="s">
+        <v>3323</v>
+      </c>
+      <c r="J5">
+        <v>3088</v>
+      </c>
+      <c r="K5">
+        <v>1400</v>
+      </c>
+      <c r="L5">
+        <v>45317</v>
+      </c>
+      <c r="M5" s="3">
+        <f>G5/L5</f>
+        <v>7.1032945693669039E-2</v>
+      </c>
+      <c r="N5" t="s">
+        <v>3328</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="1">
-        <v>44112</v>
+        <v>44120</v>
       </c>
       <c r="B6" t="s">
         <v>853</v>
@@ -10554,12 +10712,34 @@
         <v>873</v>
       </c>
       <c r="G6">
-        <v>2917</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
+        <v>3049</v>
+      </c>
+      <c r="H6" t="s">
+        <v>3322</v>
+      </c>
+      <c r="I6">
+        <v>100982</v>
+      </c>
+      <c r="J6">
+        <v>3049</v>
+      </c>
+      <c r="K6">
+        <v>1365</v>
+      </c>
+      <c r="L6">
+        <v>32621</v>
+      </c>
+      <c r="M6" s="3">
+        <f>G6/L6</f>
+        <v>9.3467398301707486E-2</v>
+      </c>
+      <c r="N6" t="s">
+        <v>3329</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="1">
-        <v>44112</v>
+        <v>44120</v>
       </c>
       <c r="B7" t="s">
         <v>453</v>
@@ -10577,12 +10757,34 @@
         <v>591</v>
       </c>
       <c r="G7">
-        <v>2908</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
+        <v>3475</v>
+      </c>
+      <c r="H7" t="s">
+        <v>3338</v>
+      </c>
+      <c r="I7" t="s">
+        <v>1214</v>
+      </c>
+      <c r="J7">
+        <v>2603</v>
+      </c>
+      <c r="K7">
+        <v>773</v>
+      </c>
+      <c r="L7">
+        <v>56567</v>
+      </c>
+      <c r="M7" s="3">
+        <f>G7/L7</f>
+        <v>6.143157671433875E-2</v>
+      </c>
+      <c r="N7" t="s">
+        <v>3341</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" s="1">
-        <v>44112</v>
+        <v>44120</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -10600,12 +10802,31 @@
         <v>72</v>
       </c>
       <c r="G8">
-        <v>2784</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
+        <v>2839</v>
+      </c>
+      <c r="H8">
+        <v>2020</v>
+      </c>
+      <c r="I8" t="s">
+        <v>1214</v>
+      </c>
+      <c r="J8">
+        <v>2578</v>
+      </c>
+      <c r="K8" t="s">
+        <v>1214</v>
+      </c>
+      <c r="L8">
+        <v>37842</v>
+      </c>
+      <c r="M8" s="3">
+        <f>G8/L8</f>
+        <v>7.5022461814914648E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" s="1">
-        <v>44112</v>
+        <v>44120</v>
       </c>
       <c r="B9" t="s">
         <v>2401</v>
@@ -10623,12 +10844,31 @@
         <v>2518</v>
       </c>
       <c r="G9">
-        <v>2682</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
+        <v>3455</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>3342</v>
+      </c>
+      <c r="I9">
+        <v>48666</v>
+      </c>
+      <c r="J9">
+        <v>3448</v>
+      </c>
+      <c r="K9">
+        <v>830</v>
+      </c>
+      <c r="L9">
+        <v>46000</v>
+      </c>
+      <c r="M9" s="3">
+        <f>G9/L9</f>
+        <v>7.5108695652173915E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="1">
-        <v>44112</v>
+        <v>44120</v>
       </c>
       <c r="B10" t="s">
         <v>746</v>
@@ -10646,12 +10886,34 @@
         <v>846</v>
       </c>
       <c r="G10">
-        <v>2621</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
+        <v>2767</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>3346</v>
+      </c>
+      <c r="I10">
+        <v>564536</v>
+      </c>
+      <c r="J10">
+        <v>2767</v>
+      </c>
+      <c r="K10">
+        <v>6273</v>
+      </c>
+      <c r="L10">
+        <v>52331</v>
+      </c>
+      <c r="M10" s="3">
+        <f>G10/L10</f>
+        <v>5.2874968947660084E-2</v>
+      </c>
+      <c r="N10" t="s">
+        <v>3347</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="1">
-        <v>44112</v>
+        <v>44120</v>
       </c>
       <c r="B11" t="s">
         <v>2654</v>
@@ -10669,10 +10931,29 @@
         <v>2691</v>
       </c>
       <c r="G11">
-        <v>2494</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17">
+        <v>2537</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>3322</v>
+      </c>
+      <c r="I11">
+        <v>28508</v>
+      </c>
+      <c r="J11">
+        <v>2477</v>
+      </c>
+      <c r="K11">
+        <v>229</v>
+      </c>
+      <c r="L11">
+        <v>35487</v>
+      </c>
+      <c r="M11" s="3">
+        <f>G11/L11</f>
+        <v>7.1490968523684736E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="1">
         <v>44112</v>
       </c>
@@ -10692,10 +10973,29 @@
         <v>124</v>
       </c>
       <c r="G12">
-        <v>2381</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
+        <v>2412</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>3348</v>
+      </c>
+      <c r="I12">
+        <v>50120</v>
+      </c>
+      <c r="J12">
+        <v>2412</v>
+      </c>
+      <c r="K12">
+        <v>651</v>
+      </c>
+      <c r="L12">
+        <v>44831</v>
+      </c>
+      <c r="M12" s="3">
+        <f>G12/L12</f>
+        <v>5.3802056612611809E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" s="1">
         <v>44112</v>
       </c>
@@ -10717,8 +11017,12 @@
       <c r="G13">
         <v>2109</v>
       </c>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="M13" s="3" t="e">
+        <f>G13/L13</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="1">
         <v>44112</v>
       </c>
@@ -10740,8 +11044,12 @@
       <c r="G14">
         <v>2070</v>
       </c>
-    </row>
-    <row r="15" spans="1:17">
+      <c r="M14" s="3" t="e">
+        <f>G14/L14</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" s="1">
         <v>44112</v>
       </c>
@@ -10763,8 +11071,12 @@
       <c r="G15">
         <v>2034</v>
       </c>
-    </row>
-    <row r="16" spans="1:17">
+      <c r="M15" s="3" t="e">
+        <f>G15/L15</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" s="1">
         <v>44112</v>
       </c>
@@ -10786,8 +11098,12 @@
       <c r="G16">
         <v>1982</v>
       </c>
-    </row>
-    <row r="17" spans="1:17">
+      <c r="M16" s="3" t="e">
+        <f>G16/L16</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" s="1">
         <v>44112</v>
       </c>
@@ -10809,8 +11125,12 @@
       <c r="G17">
         <v>1821</v>
       </c>
-    </row>
-    <row r="18" spans="1:17">
+      <c r="M17" s="3" t="e">
+        <f>G17/L17</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="1">
         <v>44112</v>
       </c>
@@ -10832,8 +11152,12 @@
       <c r="G18">
         <v>1805</v>
       </c>
-    </row>
-    <row r="19" spans="1:17">
+      <c r="M18" s="3" t="e">
+        <f>G18/L18</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="1">
         <v>44112</v>
       </c>
@@ -10855,8 +11179,12 @@
       <c r="G19">
         <v>1801</v>
       </c>
-    </row>
-    <row r="20" spans="1:17">
+      <c r="M19" s="3" t="e">
+        <f>G19/L19</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="1">
         <v>44112</v>
       </c>
@@ -10878,8 +11206,12 @@
       <c r="G20">
         <v>1799</v>
       </c>
-    </row>
-    <row r="21" spans="1:17">
+      <c r="M20" s="3" t="e">
+        <f>G20/L20</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" s="1">
         <v>44112</v>
       </c>
@@ -10901,8 +11233,12 @@
       <c r="G21">
         <v>1773</v>
       </c>
-    </row>
-    <row r="22" spans="1:17">
+      <c r="M21" s="3" t="e">
+        <f>G21/L21</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" s="1">
         <v>44112</v>
       </c>
@@ -10924,8 +11260,12 @@
       <c r="G22">
         <v>1768</v>
       </c>
-    </row>
-    <row r="23" spans="1:17">
+      <c r="M22" s="3" t="e">
+        <f>G22/L22</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" s="1">
         <v>44112</v>
       </c>
@@ -10947,8 +11287,12 @@
       <c r="G23">
         <v>1661</v>
       </c>
-    </row>
-    <row r="24" spans="1:17">
+      <c r="M23" s="3" t="e">
+        <f>G23/L23</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" s="1">
         <v>44112</v>
       </c>
@@ -10970,8 +11314,12 @@
       <c r="G24">
         <v>1656</v>
       </c>
-    </row>
-    <row r="25" spans="1:17">
+      <c r="M24" s="3" t="e">
+        <f>G24/L24</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" s="1">
         <v>44112</v>
       </c>
@@ -10993,8 +11341,12 @@
       <c r="G25">
         <v>1562</v>
       </c>
-    </row>
-    <row r="26" spans="1:17">
+      <c r="M25" s="3" t="e">
+        <f>G25/L25</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" s="1">
         <v>44112</v>
       </c>
@@ -11016,8 +11368,12 @@
       <c r="G26">
         <v>1527</v>
       </c>
-    </row>
-    <row r="27" spans="1:17">
+      <c r="M26" s="3" t="e">
+        <f>G26/L26</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" s="1">
         <v>44112</v>
       </c>
@@ -11039,8 +11395,12 @@
       <c r="G27">
         <v>1485</v>
       </c>
-    </row>
-    <row r="28" spans="1:17">
+      <c r="M27" s="3" t="e">
+        <f>G27/L27</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" s="1">
         <v>44112</v>
       </c>
@@ -11062,8 +11422,12 @@
       <c r="G28">
         <v>1420</v>
       </c>
-    </row>
-    <row r="29" spans="1:17">
+      <c r="M28" s="3" t="e">
+        <f>G28/L28</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29" s="1">
         <v>44112</v>
       </c>
@@ -11085,8 +11449,12 @@
       <c r="G29">
         <v>1384</v>
       </c>
-    </row>
-    <row r="30" spans="1:17">
+      <c r="M29" s="3" t="e">
+        <f>G29/L29</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30" s="1">
         <v>44112</v>
       </c>
@@ -11108,8 +11476,12 @@
       <c r="G30">
         <v>1361</v>
       </c>
-    </row>
-    <row r="31" spans="1:17">
+      <c r="M30" s="3" t="e">
+        <f>G30/L30</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
       <c r="A31" s="1">
         <v>44112</v>
       </c>
@@ -11131,11 +11503,15 @@
       <c r="G31">
         <v>1353</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="M31" s="3" t="e">
+        <f>G31/L31</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N31" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:14">
       <c r="A32" s="1">
         <v>44112</v>
       </c>
@@ -11157,8 +11533,12 @@
       <c r="G32">
         <v>1340</v>
       </c>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="M32" s="3" t="e">
+        <f>G32/L32</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
       <c r="A33" s="1">
         <v>44112</v>
       </c>
@@ -11180,8 +11560,12 @@
       <c r="G33">
         <v>1299</v>
       </c>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="M33" s="3" t="e">
+        <f>G33/L33</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
       <c r="A34" s="1">
         <v>44112</v>
       </c>
@@ -11203,8 +11587,12 @@
       <c r="G34">
         <v>1297</v>
       </c>
-    </row>
-    <row r="35" spans="1:7">
+      <c r="M34" s="3" t="e">
+        <f>G34/L34</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
       <c r="A35" s="1">
         <v>44112</v>
       </c>
@@ -11226,8 +11614,12 @@
       <c r="G35">
         <v>1229</v>
       </c>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="M35" s="3" t="e">
+        <f>G35/L35</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
       <c r="A36" s="1">
         <v>44112</v>
       </c>
@@ -11249,8 +11641,12 @@
       <c r="G36">
         <v>1210</v>
       </c>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="M36" s="3" t="e">
+        <f>G36/L36</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
       <c r="A37" s="1">
         <v>44112</v>
       </c>
@@ -11272,8 +11668,12 @@
       <c r="G37">
         <v>1200</v>
       </c>
-    </row>
-    <row r="38" spans="1:7">
+      <c r="M37" s="3" t="e">
+        <f>G37/L37</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
       <c r="A38" s="1">
         <v>44112</v>
       </c>
@@ -11295,8 +11695,12 @@
       <c r="G38">
         <v>1178</v>
       </c>
-    </row>
-    <row r="39" spans="1:7">
+      <c r="M38" s="3" t="e">
+        <f>G38/L38</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
       <c r="A39" s="1">
         <v>44112</v>
       </c>
@@ -11318,8 +11722,12 @@
       <c r="G39">
         <v>1167</v>
       </c>
-    </row>
-    <row r="40" spans="1:7">
+      <c r="M39" s="3" t="e">
+        <f>G39/L39</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
       <c r="A40" s="1">
         <v>44112</v>
       </c>
@@ -11341,8 +11749,12 @@
       <c r="G40">
         <v>1148</v>
       </c>
-    </row>
-    <row r="41" spans="1:7">
+      <c r="M40" s="3" t="e">
+        <f>G40/L40</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
       <c r="A41" s="1">
         <v>44112</v>
       </c>
@@ -11364,8 +11776,12 @@
       <c r="G41">
         <v>1134</v>
       </c>
-    </row>
-    <row r="42" spans="1:7">
+      <c r="M41" s="3" t="e">
+        <f>G41/L41</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
       <c r="A42" s="1">
         <v>44112</v>
       </c>
@@ -11387,8 +11803,12 @@
       <c r="G42">
         <v>1115</v>
       </c>
-    </row>
-    <row r="43" spans="1:7">
+      <c r="M42" s="3" t="e">
+        <f>G42/L42</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
       <c r="A43" s="1">
         <v>44112</v>
       </c>
@@ -11410,8 +11830,12 @@
       <c r="G43">
         <v>1102</v>
       </c>
-    </row>
-    <row r="44" spans="1:7">
+      <c r="M43" s="3" t="e">
+        <f>G43/L43</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
       <c r="A44" s="1">
         <v>44112</v>
       </c>
@@ -11433,8 +11857,12 @@
       <c r="G44">
         <v>1082</v>
       </c>
-    </row>
-    <row r="45" spans="1:7">
+      <c r="M44" s="3" t="e">
+        <f>G44/L44</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
       <c r="A45" s="1">
         <v>44112</v>
       </c>
@@ -11456,8 +11884,12 @@
       <c r="G45">
         <v>1027</v>
       </c>
-    </row>
-    <row r="46" spans="1:7">
+      <c r="M45" s="3" t="e">
+        <f>G45/L45</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
       <c r="A46" s="1">
         <v>44112</v>
       </c>
@@ -11479,8 +11911,12 @@
       <c r="G46">
         <v>1009</v>
       </c>
-    </row>
-    <row r="47" spans="1:7">
+      <c r="M46" s="3" t="e">
+        <f>G46/L46</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
       <c r="A47" s="1">
         <v>44112</v>
       </c>
@@ -11502,8 +11938,12 @@
       <c r="G47">
         <v>1008</v>
       </c>
-    </row>
-    <row r="48" spans="1:7">
+      <c r="M47" s="3" t="e">
+        <f>G47/L47</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
       <c r="A48" s="1">
         <v>44112</v>
       </c>
@@ -11525,8 +11965,12 @@
       <c r="G48">
         <v>964</v>
       </c>
-    </row>
-    <row r="49" spans="1:7">
+      <c r="M48" s="3" t="e">
+        <f>G48/L48</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
       <c r="A49" s="1">
         <v>44112</v>
       </c>
@@ -11548,8 +11992,12 @@
       <c r="G49">
         <v>929</v>
       </c>
-    </row>
-    <row r="50" spans="1:7">
+      <c r="M49" s="3" t="e">
+        <f>G49/L49</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
       <c r="A50" s="1">
         <v>44112</v>
       </c>
@@ -11571,8 +12019,12 @@
       <c r="G50">
         <v>890</v>
       </c>
-    </row>
-    <row r="51" spans="1:7">
+      <c r="M50" s="3" t="e">
+        <f>G50/L50</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13">
       <c r="A51" s="1">
         <v>44112</v>
       </c>
@@ -11594,8 +12046,12 @@
       <c r="G51">
         <v>863</v>
       </c>
-    </row>
-    <row r="52" spans="1:7">
+      <c r="M51" s="3" t="e">
+        <f>G51/L51</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
       <c r="A52" s="1">
         <v>44112</v>
       </c>
@@ -11617,8 +12073,12 @@
       <c r="G52">
         <v>844</v>
       </c>
-    </row>
-    <row r="53" spans="1:7">
+      <c r="M52" s="3" t="e">
+        <f>G52/L52</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
       <c r="A53" s="1">
         <v>44112</v>
       </c>
@@ -11640,8 +12100,12 @@
       <c r="G53">
         <v>811</v>
       </c>
-    </row>
-    <row r="54" spans="1:7">
+      <c r="M53" s="3" t="e">
+        <f>G53/L53</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
       <c r="A54" s="1">
         <v>44112</v>
       </c>
@@ -11663,8 +12127,12 @@
       <c r="G54">
         <v>787</v>
       </c>
-    </row>
-    <row r="55" spans="1:7">
+      <c r="M54" s="3" t="e">
+        <f>G54/L54</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
       <c r="A55" s="1">
         <v>44112</v>
       </c>
@@ -11686,8 +12154,12 @@
       <c r="G55">
         <v>782</v>
       </c>
-    </row>
-    <row r="56" spans="1:7">
+      <c r="M55" s="3" t="e">
+        <f>G55/L55</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
       <c r="A56" s="1">
         <v>44112</v>
       </c>
@@ -11709,8 +12181,12 @@
       <c r="G56">
         <v>735</v>
       </c>
-    </row>
-    <row r="57" spans="1:7">
+      <c r="M56" s="3" t="e">
+        <f>G56/L56</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13">
       <c r="A57" s="1">
         <v>44112</v>
       </c>
@@ -11732,8 +12208,12 @@
       <c r="G57">
         <v>734</v>
       </c>
-    </row>
-    <row r="58" spans="1:7">
+      <c r="M57" s="3" t="e">
+        <f>G57/L57</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13">
       <c r="A58" s="1">
         <v>44112</v>
       </c>
@@ -11755,8 +12235,12 @@
       <c r="G58">
         <v>724</v>
       </c>
-    </row>
-    <row r="59" spans="1:7">
+      <c r="M58" s="3" t="e">
+        <f>G58/L58</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13">
       <c r="A59" s="1">
         <v>44112</v>
       </c>
@@ -11778,8 +12262,12 @@
       <c r="G59">
         <v>707</v>
       </c>
-    </row>
-    <row r="60" spans="1:7">
+      <c r="M59" s="3" t="e">
+        <f>G59/L59</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13">
       <c r="A60" s="1">
         <v>44112</v>
       </c>
@@ -11801,8 +12289,12 @@
       <c r="G60">
         <v>701</v>
       </c>
-    </row>
-    <row r="61" spans="1:7">
+      <c r="M60" s="3" t="e">
+        <f>G60/L60</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13">
       <c r="A61" s="1">
         <v>44112</v>
       </c>
@@ -11824,8 +12316,12 @@
       <c r="G61">
         <v>700</v>
       </c>
-    </row>
-    <row r="62" spans="1:7">
+      <c r="M61" s="3" t="e">
+        <f>G61/L61</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13">
       <c r="A62" s="1">
         <v>44112</v>
       </c>
@@ -11847,8 +12343,12 @@
       <c r="G62">
         <v>694</v>
       </c>
-    </row>
-    <row r="63" spans="1:7">
+      <c r="M62" s="3" t="e">
+        <f>G62/L62</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13">
       <c r="A63" s="1">
         <v>44112</v>
       </c>
@@ -11870,8 +12370,12 @@
       <c r="G63">
         <v>674</v>
       </c>
-    </row>
-    <row r="64" spans="1:7">
+      <c r="M63" s="3" t="e">
+        <f>G63/L63</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13">
       <c r="A64" s="1">
         <v>44112</v>
       </c>
@@ -11893,8 +12397,12 @@
       <c r="G64">
         <v>665</v>
       </c>
-    </row>
-    <row r="65" spans="1:17">
+      <c r="M64" s="3" t="e">
+        <f>G64/L64</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14">
       <c r="A65" s="1">
         <v>44112</v>
       </c>
@@ -11916,8 +12424,12 @@
       <c r="G65">
         <v>642</v>
       </c>
-    </row>
-    <row r="66" spans="1:17">
+      <c r="M65" s="3" t="e">
+        <f>G65/L65</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14">
       <c r="A66" s="1">
         <v>44112</v>
       </c>
@@ -11939,8 +12451,12 @@
       <c r="G66">
         <v>638</v>
       </c>
-    </row>
-    <row r="67" spans="1:17">
+      <c r="M66" s="3" t="e">
+        <f>G66/L66</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14">
       <c r="A67" s="1">
         <v>44112</v>
       </c>
@@ -11962,8 +12478,12 @@
       <c r="G67">
         <v>638</v>
       </c>
-    </row>
-    <row r="68" spans="1:17">
+      <c r="M67" s="3" t="e">
+        <f>G67/L67</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14">
       <c r="A68" s="1">
         <v>44112</v>
       </c>
@@ -11985,8 +12505,12 @@
       <c r="G68">
         <v>623</v>
       </c>
-    </row>
-    <row r="69" spans="1:17">
+      <c r="M68" s="3" t="e">
+        <f>G68/L68</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14">
       <c r="A69" s="1">
         <v>44112</v>
       </c>
@@ -12008,8 +12532,12 @@
       <c r="G69">
         <v>588</v>
       </c>
-    </row>
-    <row r="70" spans="1:17">
+      <c r="M69" s="3" t="e">
+        <f>G69/L69</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14">
       <c r="A70" s="1">
         <v>44112</v>
       </c>
@@ -12031,8 +12559,12 @@
       <c r="G70">
         <v>585</v>
       </c>
-    </row>
-    <row r="71" spans="1:17">
+      <c r="M70" s="3" t="e">
+        <f>G70/L70</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14">
       <c r="A71" s="1">
         <v>44112</v>
       </c>
@@ -12054,8 +12586,12 @@
       <c r="G71">
         <v>568</v>
       </c>
-    </row>
-    <row r="72" spans="1:17">
+      <c r="M71" s="3" t="e">
+        <f>G71/L71</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14">
       <c r="A72" s="1">
         <v>44112</v>
       </c>
@@ -12077,11 +12613,15 @@
       <c r="G72">
         <v>550</v>
       </c>
-      <c r="Q72" t="s">
+      <c r="M72" s="3" t="e">
+        <f>G72/L72</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N72" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="73" spans="1:17">
+    <row r="73" spans="1:14">
       <c r="A73" s="1">
         <v>44112</v>
       </c>
@@ -12103,8 +12643,12 @@
       <c r="G73">
         <v>548</v>
       </c>
-    </row>
-    <row r="74" spans="1:17">
+      <c r="M73" s="3" t="e">
+        <f>G73/L73</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14">
       <c r="A74" s="1">
         <v>44112</v>
       </c>
@@ -12126,8 +12670,12 @@
       <c r="G74">
         <v>542</v>
       </c>
-    </row>
-    <row r="75" spans="1:17">
+      <c r="M74" s="3" t="e">
+        <f>G74/L74</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14">
       <c r="A75" s="1">
         <v>44112</v>
       </c>
@@ -12149,8 +12697,12 @@
       <c r="G75">
         <v>536</v>
       </c>
-    </row>
-    <row r="76" spans="1:17">
+      <c r="M75" s="3" t="e">
+        <f>G75/L75</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14">
       <c r="A76" s="1">
         <v>44112</v>
       </c>
@@ -12172,8 +12724,12 @@
       <c r="G76">
         <v>528</v>
       </c>
-    </row>
-    <row r="77" spans="1:17">
+      <c r="M76" s="3" t="e">
+        <f>G76/L76</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="77" spans="1:14">
       <c r="A77" s="1">
         <v>44112</v>
       </c>
@@ -12195,8 +12751,12 @@
       <c r="G77">
         <v>528</v>
       </c>
-    </row>
-    <row r="78" spans="1:17">
+      <c r="M77" s="3" t="e">
+        <f>G77/L77</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="78" spans="1:14">
       <c r="A78" s="1">
         <v>44112</v>
       </c>
@@ -12218,8 +12778,12 @@
       <c r="G78">
         <v>527</v>
       </c>
-    </row>
-    <row r="79" spans="1:17">
+      <c r="M78" s="3" t="e">
+        <f>G78/L78</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="79" spans="1:14">
       <c r="A79" s="1">
         <v>44112</v>
       </c>
@@ -12241,8 +12805,12 @@
       <c r="G79">
         <v>516</v>
       </c>
-    </row>
-    <row r="80" spans="1:17">
+      <c r="M79" s="3" t="e">
+        <f>G79/L79</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="80" spans="1:14">
       <c r="A80" s="1">
         <v>44112</v>
       </c>
@@ -12264,8 +12832,12 @@
       <c r="G80">
         <v>515</v>
       </c>
-    </row>
-    <row r="81" spans="1:7">
+      <c r="M80" s="3" t="e">
+        <f>G80/L80</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13">
       <c r="A81" s="1">
         <v>44112</v>
       </c>
@@ -12287,8 +12859,12 @@
       <c r="G81">
         <v>506</v>
       </c>
-    </row>
-    <row r="82" spans="1:7">
+      <c r="M81" s="3" t="e">
+        <f>G81/L81</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13">
       <c r="A82" s="1">
         <v>44112</v>
       </c>
@@ -12310,8 +12886,12 @@
       <c r="G82">
         <v>503</v>
       </c>
-    </row>
-    <row r="83" spans="1:7">
+      <c r="M82" s="3" t="e">
+        <f>G82/L82</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13">
       <c r="A83" s="1">
         <v>44112</v>
       </c>
@@ -12333,8 +12913,12 @@
       <c r="G83">
         <v>498</v>
       </c>
-    </row>
-    <row r="84" spans="1:7">
+      <c r="M83" s="3" t="e">
+        <f>G83/L83</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13">
       <c r="A84" s="1">
         <v>44112</v>
       </c>
@@ -12356,8 +12940,12 @@
       <c r="G84">
         <v>494</v>
       </c>
-    </row>
-    <row r="85" spans="1:7">
+      <c r="M84" s="3" t="e">
+        <f>G84/L84</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13">
       <c r="A85" s="1">
         <v>44112</v>
       </c>
@@ -12379,8 +12967,12 @@
       <c r="G85">
         <v>491</v>
       </c>
-    </row>
-    <row r="86" spans="1:7">
+      <c r="M85" s="3" t="e">
+        <f>G85/L85</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13">
       <c r="A86" s="1">
         <v>44112</v>
       </c>
@@ -12402,8 +12994,12 @@
       <c r="G86">
         <v>485</v>
       </c>
-    </row>
-    <row r="87" spans="1:7">
+      <c r="M86" s="3" t="e">
+        <f>G86/L86</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13">
       <c r="A87" s="1">
         <v>44112</v>
       </c>
@@ -12425,8 +13021,12 @@
       <c r="G87">
         <v>479</v>
       </c>
-    </row>
-    <row r="88" spans="1:7">
+      <c r="M87" s="3" t="e">
+        <f>G87/L87</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13">
       <c r="A88" s="1">
         <v>44112</v>
       </c>
@@ -12448,8 +13048,12 @@
       <c r="G88">
         <v>478</v>
       </c>
-    </row>
-    <row r="89" spans="1:7">
+      <c r="M88" s="3" t="e">
+        <f>G88/L88</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13">
       <c r="A89" s="1">
         <v>44112</v>
       </c>
@@ -12471,8 +13075,12 @@
       <c r="G89">
         <v>476</v>
       </c>
-    </row>
-    <row r="90" spans="1:7">
+      <c r="M89" s="3" t="e">
+        <f>G89/L89</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13">
       <c r="A90" s="1">
         <v>44112</v>
       </c>
@@ -12494,8 +13102,12 @@
       <c r="G90">
         <v>468</v>
       </c>
-    </row>
-    <row r="91" spans="1:7">
+      <c r="M90" s="3" t="e">
+        <f>G90/L90</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13">
       <c r="A91" s="1">
         <v>44112</v>
       </c>
@@ -12517,8 +13129,12 @@
       <c r="G91">
         <v>459</v>
       </c>
-    </row>
-    <row r="92" spans="1:7">
+      <c r="M91" s="3" t="e">
+        <f>G91/L91</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13">
       <c r="A92" s="1">
         <v>44112</v>
       </c>
@@ -12540,8 +13156,12 @@
       <c r="G92">
         <v>456</v>
       </c>
-    </row>
-    <row r="93" spans="1:7">
+      <c r="M92" s="3" t="e">
+        <f>G92/L92</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13">
       <c r="A93" s="1">
         <v>44112</v>
       </c>
@@ -12563,8 +13183,12 @@
       <c r="G93">
         <v>443</v>
       </c>
-    </row>
-    <row r="94" spans="1:7">
+      <c r="M93" s="3" t="e">
+        <f>G93/L93</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13">
       <c r="A94" s="1">
         <v>44112</v>
       </c>
@@ -12586,8 +13210,12 @@
       <c r="G94">
         <v>436</v>
       </c>
-    </row>
-    <row r="95" spans="1:7">
+      <c r="M94" s="3" t="e">
+        <f>G94/L94</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13">
       <c r="A95" s="1">
         <v>44112</v>
       </c>
@@ -12609,8 +13237,12 @@
       <c r="G95">
         <v>436</v>
       </c>
-    </row>
-    <row r="96" spans="1:7">
+      <c r="M95" s="3" t="e">
+        <f>G95/L95</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13">
       <c r="A96" s="1">
         <v>44112</v>
       </c>
@@ -12632,8 +13264,12 @@
       <c r="G96">
         <v>421</v>
       </c>
-    </row>
-    <row r="97" spans="1:7">
+      <c r="M96" s="3" t="e">
+        <f>G96/L96</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13">
       <c r="A97" s="1">
         <v>44112</v>
       </c>
@@ -12655,8 +13291,12 @@
       <c r="G97">
         <v>414</v>
       </c>
-    </row>
-    <row r="98" spans="1:7">
+      <c r="M97" s="3" t="e">
+        <f>G97/L97</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13">
       <c r="A98" s="1">
         <v>44112</v>
       </c>
@@ -12678,8 +13318,12 @@
       <c r="G98">
         <v>413</v>
       </c>
-    </row>
-    <row r="99" spans="1:7">
+      <c r="M98" s="3" t="e">
+        <f>G98/L98</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13">
       <c r="A99" s="1">
         <v>44112</v>
       </c>
@@ -12701,8 +13345,12 @@
       <c r="G99">
         <v>408</v>
       </c>
-    </row>
-    <row r="100" spans="1:7">
+      <c r="M99" s="3" t="e">
+        <f>G99/L99</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13">
       <c r="A100" s="1">
         <v>44112</v>
       </c>
@@ -12724,8 +13372,12 @@
       <c r="G100">
         <v>408</v>
       </c>
-    </row>
-    <row r="101" spans="1:7">
+      <c r="M100" s="3" t="e">
+        <f>G100/L100</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13">
       <c r="A101" s="1">
         <v>44112</v>
       </c>
@@ -12748,7 +13400,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:13">
       <c r="A102" s="1">
         <v>44112</v>
       </c>
@@ -12771,7 +13423,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:13">
       <c r="A103" s="1">
         <v>44112</v>
       </c>
@@ -12794,7 +13446,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="104" spans="1:7">
+    <row r="104" spans="1:13">
       <c r="A104" s="1">
         <v>44112</v>
       </c>
@@ -12817,7 +13469,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:13">
       <c r="A105" s="1">
         <v>44112</v>
       </c>
@@ -12840,7 +13492,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:13">
       <c r="A106" s="1">
         <v>44112</v>
       </c>
@@ -12863,7 +13515,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:13">
       <c r="A107" s="1">
         <v>44112</v>
       </c>
@@ -12886,7 +13538,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:13">
       <c r="A108" s="1">
         <v>44112</v>
       </c>
@@ -12909,7 +13561,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:13">
       <c r="A109" s="1">
         <v>44112</v>
       </c>
@@ -12932,7 +13584,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:13">
       <c r="A110" s="1">
         <v>44112</v>
       </c>
@@ -12955,7 +13607,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:13">
       <c r="A111" s="1">
         <v>44112</v>
       </c>
@@ -12978,7 +13630,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:13">
       <c r="A112" s="1">
         <v>44112</v>
       </c>
@@ -13001,7 +13653,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="113" spans="1:17">
+    <row r="113" spans="1:14">
       <c r="A113" s="1">
         <v>44112</v>
       </c>
@@ -13024,7 +13676,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="114" spans="1:17">
+    <row r="114" spans="1:14">
       <c r="A114" s="1">
         <v>44112</v>
       </c>
@@ -13047,7 +13699,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="115" spans="1:17">
+    <row r="115" spans="1:14">
       <c r="A115" s="1">
         <v>44112</v>
       </c>
@@ -13069,11 +13721,11 @@
       <c r="G115">
         <v>332</v>
       </c>
-      <c r="Q115" t="s">
+      <c r="N115" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="116" spans="1:17">
+    <row r="116" spans="1:14">
       <c r="A116" s="1">
         <v>44112</v>
       </c>
@@ -13096,7 +13748,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="117" spans="1:17">
+    <row r="117" spans="1:14">
       <c r="A117" s="1">
         <v>44112</v>
       </c>
@@ -13119,7 +13771,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="118" spans="1:17">
+    <row r="118" spans="1:14">
       <c r="A118" s="1">
         <v>44112</v>
       </c>
@@ -13142,7 +13794,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="119" spans="1:17">
+    <row r="119" spans="1:14">
       <c r="A119" s="1">
         <v>44112</v>
       </c>
@@ -13165,7 +13817,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="120" spans="1:17">
+    <row r="120" spans="1:14">
       <c r="A120" s="1">
         <v>44112</v>
       </c>
@@ -13188,7 +13840,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="121" spans="1:17">
+    <row r="121" spans="1:14">
       <c r="A121" s="1">
         <v>44112</v>
       </c>
@@ -13211,7 +13863,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="122" spans="1:17">
+    <row r="122" spans="1:14">
       <c r="A122" s="1">
         <v>44112</v>
       </c>
@@ -13234,7 +13886,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="123" spans="1:17">
+    <row r="123" spans="1:14">
       <c r="A123" s="1">
         <v>44112</v>
       </c>
@@ -13257,7 +13909,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="124" spans="1:17">
+    <row r="124" spans="1:14">
       <c r="A124" s="1">
         <v>44112</v>
       </c>
@@ -13280,7 +13932,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="125" spans="1:17">
+    <row r="125" spans="1:14">
       <c r="A125" s="1">
         <v>44112</v>
       </c>
@@ -13303,7 +13955,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="126" spans="1:17">
+    <row r="126" spans="1:14">
       <c r="A126" s="1">
         <v>44112</v>
       </c>
@@ -13326,7 +13978,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="127" spans="1:17">
+    <row r="127" spans="1:14">
       <c r="A127" s="1">
         <v>44112</v>
       </c>
@@ -13349,7 +14001,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="128" spans="1:17">
+    <row r="128" spans="1:14">
       <c r="A128" s="1">
         <v>44112</v>
       </c>
@@ -13372,7 +14024,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="129" spans="1:17">
+    <row r="129" spans="1:14">
       <c r="A129" s="1">
         <v>44112</v>
       </c>
@@ -13395,7 +14047,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="130" spans="1:17">
+    <row r="130" spans="1:14">
       <c r="A130" s="1">
         <v>44112</v>
       </c>
@@ -13418,7 +14070,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="131" spans="1:17">
+    <row r="131" spans="1:14">
       <c r="A131" s="1">
         <v>44112</v>
       </c>
@@ -13440,11 +14092,11 @@
       <c r="G131">
         <v>300</v>
       </c>
-      <c r="Q131" t="s">
+      <c r="N131" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="132" spans="1:17">
+    <row r="132" spans="1:14">
       <c r="A132" s="1">
         <v>44112</v>
       </c>
@@ -13467,7 +14119,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="133" spans="1:17">
+    <row r="133" spans="1:14">
       <c r="A133" s="1">
         <v>44112</v>
       </c>
@@ -13490,7 +14142,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="134" spans="1:17">
+    <row r="134" spans="1:14">
       <c r="A134" s="1">
         <v>44112</v>
       </c>
@@ -13513,7 +14165,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="135" spans="1:17">
+    <row r="135" spans="1:14">
       <c r="A135" s="1">
         <v>44112</v>
       </c>
@@ -13536,7 +14188,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="136" spans="1:17">
+    <row r="136" spans="1:14">
       <c r="A136" s="1">
         <v>44112</v>
       </c>
@@ -13559,7 +14211,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="137" spans="1:17">
+    <row r="137" spans="1:14">
       <c r="A137" s="1">
         <v>44112</v>
       </c>
@@ -13582,7 +14234,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="138" spans="1:17">
+    <row r="138" spans="1:14">
       <c r="A138" s="1">
         <v>44112</v>
       </c>
@@ -13605,7 +14257,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="139" spans="1:17">
+    <row r="139" spans="1:14">
       <c r="A139" s="1">
         <v>44112</v>
       </c>
@@ -13628,7 +14280,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="140" spans="1:17">
+    <row r="140" spans="1:14">
       <c r="A140" s="1">
         <v>44112</v>
       </c>
@@ -13651,7 +14303,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="141" spans="1:17">
+    <row r="141" spans="1:14">
       <c r="A141" s="1">
         <v>44112</v>
       </c>
@@ -13674,7 +14326,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="142" spans="1:17">
+    <row r="142" spans="1:14">
       <c r="A142" s="1">
         <v>44112</v>
       </c>
@@ -13697,7 +14349,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="143" spans="1:17">
+    <row r="143" spans="1:14">
       <c r="A143" s="1">
         <v>44112</v>
       </c>
@@ -13720,7 +14372,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="144" spans="1:17">
+    <row r="144" spans="1:14">
       <c r="A144" s="1">
         <v>44112</v>
       </c>
@@ -21836,7 +22488,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="497" spans="1:17">
+    <row r="497" spans="1:14">
       <c r="A497" s="1">
         <v>44112</v>
       </c>
@@ -21859,7 +22511,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="498" spans="1:17">
+    <row r="498" spans="1:14">
       <c r="A498" s="1">
         <v>44112</v>
       </c>
@@ -21882,7 +22534,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="499" spans="1:17">
+    <row r="499" spans="1:14">
       <c r="A499" s="1">
         <v>44112</v>
       </c>
@@ -21905,7 +22557,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="500" spans="1:17">
+    <row r="500" spans="1:14">
       <c r="A500" s="1">
         <v>44112</v>
       </c>
@@ -21928,7 +22580,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="501" spans="1:17">
+    <row r="501" spans="1:14">
       <c r="A501" s="1">
         <v>44112</v>
       </c>
@@ -21951,7 +22603,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="502" spans="1:17">
+    <row r="502" spans="1:14">
       <c r="A502" s="1">
         <v>44112</v>
       </c>
@@ -21974,7 +22626,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="503" spans="1:17">
+    <row r="503" spans="1:14">
       <c r="A503" s="1">
         <v>44112</v>
       </c>
@@ -21997,7 +22649,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="504" spans="1:17">
+    <row r="504" spans="1:14">
       <c r="A504" s="1">
         <v>44112</v>
       </c>
@@ -22020,7 +22672,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="505" spans="1:17">
+    <row r="505" spans="1:14">
       <c r="A505" s="1">
         <v>44112</v>
       </c>
@@ -22043,7 +22695,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="506" spans="1:17">
+    <row r="506" spans="1:14">
       <c r="A506" s="1">
         <v>44112</v>
       </c>
@@ -22066,7 +22718,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="507" spans="1:17">
+    <row r="507" spans="1:14">
       <c r="A507" s="1">
         <v>44112</v>
       </c>
@@ -22089,7 +22741,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="508" spans="1:17">
+    <row r="508" spans="1:14">
       <c r="A508" s="1">
         <v>44112</v>
       </c>
@@ -22111,11 +22763,11 @@
       <c r="G508">
         <v>43</v>
       </c>
-      <c r="Q508" t="s">
+      <c r="N508" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="509" spans="1:17">
+    <row r="509" spans="1:14">
       <c r="A509" s="1">
         <v>44112</v>
       </c>
@@ -22138,7 +22790,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="510" spans="1:17">
+    <row r="510" spans="1:14">
       <c r="A510" s="1">
         <v>44112</v>
       </c>
@@ -22161,7 +22813,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="511" spans="1:17">
+    <row r="511" spans="1:14">
       <c r="A511" s="1">
         <v>44112</v>
       </c>
@@ -22184,7 +22836,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="512" spans="1:17">
+    <row r="512" spans="1:14">
       <c r="A512" s="1">
         <v>44112</v>
       </c>
@@ -25887,7 +26539,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="673" spans="1:17">
+    <row r="673" spans="1:14">
       <c r="A673" s="1">
         <v>44112</v>
       </c>
@@ -25910,7 +26562,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="674" spans="1:17">
+    <row r="674" spans="1:14">
       <c r="A674" s="1">
         <v>44112</v>
       </c>
@@ -25933,7 +26585,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="675" spans="1:17">
+    <row r="675" spans="1:14">
       <c r="A675" s="1">
         <v>44112</v>
       </c>
@@ -25956,7 +26608,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="676" spans="1:17">
+    <row r="676" spans="1:14">
       <c r="A676" s="1">
         <v>44112</v>
       </c>
@@ -25979,7 +26631,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="677" spans="1:17">
+    <row r="677" spans="1:14">
       <c r="A677" s="1">
         <v>44112</v>
       </c>
@@ -26002,7 +26654,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="678" spans="1:17">
+    <row r="678" spans="1:14">
       <c r="A678" s="1">
         <v>44112</v>
       </c>
@@ -26025,7 +26677,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="679" spans="1:17">
+    <row r="679" spans="1:14">
       <c r="A679" s="1">
         <v>44112</v>
       </c>
@@ -26048,7 +26700,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="680" spans="1:17">
+    <row r="680" spans="1:14">
       <c r="A680" s="1">
         <v>44112</v>
       </c>
@@ -26071,7 +26723,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="681" spans="1:17">
+    <row r="681" spans="1:14">
       <c r="A681" s="1">
         <v>44112</v>
       </c>
@@ -26094,7 +26746,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="682" spans="1:17">
+    <row r="682" spans="1:14">
       <c r="A682" s="1">
         <v>44112</v>
       </c>
@@ -26116,11 +26768,11 @@
       <c r="G682">
         <v>25</v>
       </c>
-      <c r="Q682" t="s">
+      <c r="N682" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="683" spans="1:17">
+    <row r="683" spans="1:14">
       <c r="A683" s="1">
         <v>44112</v>
       </c>
@@ -26143,7 +26795,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="684" spans="1:17">
+    <row r="684" spans="1:14">
       <c r="A684" s="1">
         <v>44112</v>
       </c>
@@ -26166,7 +26818,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="685" spans="1:17">
+    <row r="685" spans="1:14">
       <c r="A685" s="1">
         <v>44112</v>
       </c>
@@ -26189,7 +26841,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="686" spans="1:17">
+    <row r="686" spans="1:14">
       <c r="A686" s="1">
         <v>44112</v>
       </c>
@@ -26212,7 +26864,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="687" spans="1:17">
+    <row r="687" spans="1:14">
       <c r="A687" s="1">
         <v>44112</v>
       </c>
@@ -26235,7 +26887,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="688" spans="1:17">
+    <row r="688" spans="1:14">
       <c r="A688" s="1">
         <v>44112</v>
       </c>
@@ -49393,9 +50045,756 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q1713">
-    <sortCondition descending="1" ref="G2:G1713"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N1713">
+    <sortCondition descending="1" ref="G3:G1713"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{114D2CD2-0900-2B47-934E-E13A8CBAEAF3}">
+  <dimension ref="A1:H58"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1">
+        <f>1680+174</f>
+        <v>1854</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2">
+        <f>1968+227</f>
+        <v>2195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3">
+        <f>1396+128</f>
+        <v>1524</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <f>507+83</f>
+        <v>590</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <f>403+110</f>
+        <v>513</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <f>1256+148</f>
+        <v>1404</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <f>1534+189</f>
+        <v>1723</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <f>SUM(A1:A7)</f>
+        <v>9803</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <f>A8/7</f>
+        <v>1400.4285714285713</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <f>8830</f>
+        <v>8830</v>
+      </c>
+      <c r="B11">
+        <v>98</v>
+      </c>
+      <c r="C11">
+        <f>SUM(A11:B11)</f>
+        <v>8928</v>
+      </c>
+      <c r="D11">
+        <v>165</v>
+      </c>
+      <c r="E11">
+        <v>44</v>
+      </c>
+      <c r="F11">
+        <f>SUM(A11,B11,D11,E11)</f>
+        <v>9137</v>
+      </c>
+      <c r="G11">
+        <f>F11/7</f>
+        <v>1305.2857142857142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <f>9691</f>
+        <v>9691</v>
+      </c>
+      <c r="B12">
+        <v>103</v>
+      </c>
+      <c r="C12">
+        <f t="shared" ref="C12:C17" si="0">SUM(A12:B12)</f>
+        <v>9794</v>
+      </c>
+      <c r="D12">
+        <v>127</v>
+      </c>
+      <c r="E12">
+        <v>25</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ref="F12:F17" si="1">SUM(A12,B12,D12,E12)</f>
+        <v>9946</v>
+      </c>
+      <c r="G12">
+        <f t="shared" ref="G12:G17" si="2">F12/7</f>
+        <v>1420.8571428571429</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <f>9690</f>
+        <v>9690</v>
+      </c>
+      <c r="B13">
+        <v>141</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>9831</v>
+      </c>
+      <c r="D13">
+        <v>161</v>
+      </c>
+      <c r="E13">
+        <v>39</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>10031</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>1433</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <f>10190</f>
+        <v>10190</v>
+      </c>
+      <c r="B14">
+        <v>226</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>10416</v>
+      </c>
+      <c r="D14">
+        <v>187</v>
+      </c>
+      <c r="E14">
+        <v>75</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>10678</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="2"/>
+        <v>1525.4285714285713</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15">
+        <f>7225</f>
+        <v>7225</v>
+      </c>
+      <c r="B15">
+        <v>345</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>7570</v>
+      </c>
+      <c r="D15">
+        <v>298</v>
+      </c>
+      <c r="E15">
+        <v>212</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>8080</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>1154.2857142857142</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16">
+        <f>9373</f>
+        <v>9373</v>
+      </c>
+      <c r="B16">
+        <v>734</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>10107</v>
+      </c>
+      <c r="D16">
+        <v>275</v>
+      </c>
+      <c r="E16">
+        <v>260</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>10642</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="2"/>
+        <v>1520.2857142857142</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17">
+        <f>7864</f>
+        <v>7864</v>
+      </c>
+      <c r="B17">
+        <v>274</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>8138</v>
+      </c>
+      <c r="D17">
+        <v>127</v>
+      </c>
+      <c r="E17">
+        <v>108</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="1"/>
+        <v>8373</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="2"/>
+        <v>1196.1428571428571</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="C18">
+        <f>SUM(C11:C17)/7</f>
+        <v>9254.8571428571431</v>
+      </c>
+      <c r="F18">
+        <f>SUM(F11:F17)/7</f>
+        <v>9555.2857142857138</v>
+      </c>
+      <c r="G18">
+        <f>SUM(G11:G17)/7</f>
+        <v>1365.0408163265306</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="C19" t="s">
+        <v>3325</v>
+      </c>
+      <c r="F19" t="s">
+        <v>3327</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="G20" t="s">
+        <v>3326</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22">
+        <v>6563</v>
+      </c>
+      <c r="B22">
+        <f>A22/7</f>
+        <v>937.57142857142856</v>
+      </c>
+      <c r="C22" t="s">
+        <v>3335</v>
+      </c>
+      <c r="G22">
+        <v>3844</v>
+      </c>
+      <c r="H22">
+        <f>G22/7</f>
+        <v>549.14285714285711</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23">
+        <v>9172</v>
+      </c>
+      <c r="B23">
+        <f t="shared" ref="B23:B25" si="3">A23/7</f>
+        <v>1310.2857142857142</v>
+      </c>
+      <c r="G23">
+        <v>4654</v>
+      </c>
+      <c r="H23">
+        <f t="shared" ref="H23:H32" si="4">G23/7</f>
+        <v>664.85714285714289</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24">
+        <v>8725</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="3"/>
+        <v>1246.4285714285713</v>
+      </c>
+      <c r="G24">
+        <v>4988</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="4"/>
+        <v>712.57142857142856</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25">
+        <v>7698</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="3"/>
+        <v>1099.7142857142858</v>
+      </c>
+      <c r="G25">
+        <v>4961</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="4"/>
+        <v>708.71428571428567</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="B26">
+        <f>SUM(B22:B25)/4</f>
+        <v>1148.5</v>
+      </c>
+      <c r="G26">
+        <v>6987</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="4"/>
+        <v>998.14285714285711</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="G27">
+        <v>6642</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="4"/>
+        <v>948.85714285714289</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="A28">
+        <v>1655</v>
+      </c>
+      <c r="B28">
+        <f>A28/7</f>
+        <v>236.42857142857142</v>
+      </c>
+      <c r="C28" t="s">
+        <v>3340</v>
+      </c>
+      <c r="G28">
+        <v>6297</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="4"/>
+        <v>899.57142857142856</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29">
+        <v>1974</v>
+      </c>
+      <c r="B29">
+        <f t="shared" ref="B29:B32" si="5">A29/7</f>
+        <v>282</v>
+      </c>
+      <c r="G29">
+        <v>3317</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="4"/>
+        <v>473.85714285714283</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30">
+        <v>1490</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="5"/>
+        <v>212.85714285714286</v>
+      </c>
+      <c r="G30">
+        <v>5801</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="4"/>
+        <v>828.71428571428567</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31">
+        <v>1365</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="5"/>
+        <v>195</v>
+      </c>
+      <c r="G31">
+        <v>2216</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="4"/>
+        <v>316.57142857142856</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32">
+        <v>1944</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="5"/>
+        <v>277.71428571428572</v>
+      </c>
+      <c r="G32">
+        <v>413</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="4"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
+      <c r="B33">
+        <f>SUM(B28:B32)/5</f>
+        <v>240.8</v>
+      </c>
+      <c r="H33">
+        <f>AVERAGE(H22:H32)</f>
+        <v>650.90909090909088</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="A35">
+        <v>1113</v>
+      </c>
+      <c r="B35">
+        <v>55</v>
+      </c>
+      <c r="C35">
+        <f>A35+B35</f>
+        <v>1168</v>
+      </c>
+      <c r="D35" t="s">
+        <v>3339</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="A36">
+        <v>1110</v>
+      </c>
+      <c r="B36">
+        <v>62</v>
+      </c>
+      <c r="C36">
+        <f t="shared" ref="C36:C41" si="6">A36+B36</f>
+        <v>1172</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="A37">
+        <v>446</v>
+      </c>
+      <c r="B37">
+        <v>26</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="6"/>
+        <v>472</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="A38">
+        <v>400</v>
+      </c>
+      <c r="B38">
+        <v>14</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="6"/>
+        <v>414</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="A39">
+        <v>159</v>
+      </c>
+      <c r="B39">
+        <v>5</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="6"/>
+        <v>164</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
+      <c r="A40">
+        <v>763</v>
+      </c>
+      <c r="B40">
+        <v>41</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="6"/>
+        <v>804</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41">
+        <v>1168</v>
+      </c>
+      <c r="B41">
+        <v>51</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="6"/>
+        <v>1219</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="C42">
+        <f>SUM(C35:C41)/7</f>
+        <v>773.28571428571433</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="A44">
+        <f>2600+211</f>
+        <v>2811</v>
+      </c>
+      <c r="B44">
+        <f>1708+463</f>
+        <v>2171</v>
+      </c>
+      <c r="C44">
+        <f>A44+B44</f>
+        <v>4982</v>
+      </c>
+      <c r="D44">
+        <f>C44/7</f>
+        <v>711.71428571428567</v>
+      </c>
+      <c r="E44" t="s">
+        <v>3343</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="A45">
+        <v>3159</v>
+      </c>
+      <c r="B45">
+        <v>3267</v>
+      </c>
+      <c r="C45">
+        <f t="shared" ref="C45:C51" si="7">A45+B45</f>
+        <v>6426</v>
+      </c>
+      <c r="D45">
+        <f t="shared" ref="D45:D51" si="8">C45/7</f>
+        <v>918</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="A46">
+        <v>3381</v>
+      </c>
+      <c r="B46">
+        <v>2821</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="7"/>
+        <v>6202</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="8"/>
+        <v>886</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8">
+      <c r="A47">
+        <v>3359</v>
+      </c>
+      <c r="B47">
+        <v>3353</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="7"/>
+        <v>6712</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="8"/>
+        <v>958.85714285714289</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48">
+        <v>3327</v>
+      </c>
+      <c r="B48">
+        <v>3056</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="7"/>
+        <v>6383</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="8"/>
+        <v>911.85714285714289</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49">
+        <v>3176</v>
+      </c>
+      <c r="B49">
+        <v>3118</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="7"/>
+        <v>6294</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="8"/>
+        <v>899.14285714285711</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50">
+        <v>3435</v>
+      </c>
+      <c r="B50">
+        <v>1858</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="7"/>
+        <v>5293</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="8"/>
+        <v>756.14285714285711</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51">
+        <v>4020</v>
+      </c>
+      <c r="B51">
+        <v>160</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="7"/>
+        <v>4180</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="8"/>
+        <v>597.14285714285711</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="C52">
+        <f>SUM(C44:C51)/8</f>
+        <v>5809</v>
+      </c>
+      <c r="D52">
+        <f>SUM(D44:D51)/8</f>
+        <v>829.85714285714278</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="C53" t="s">
+        <v>3344</v>
+      </c>
+      <c r="D53" t="s">
+        <v>3345</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55">
+        <v>1025</v>
+      </c>
+      <c r="B55">
+        <f>A55/7</f>
+        <v>146.42857142857142</v>
+      </c>
+      <c r="C55" t="s">
+        <v>3349</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56">
+        <v>2623</v>
+      </c>
+      <c r="B56">
+        <f t="shared" ref="B56:B57" si="9">A56/7</f>
+        <v>374.71428571428572</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57">
+        <v>1154</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="9"/>
+        <v>164.85714285714286</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="B58">
+        <f>SUM(B55:B57)/3</f>
+        <v>228.66666666666666</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>